<commit_message>
task #3 Fix case 'not equal' and inhomogeneous types and Test more cases
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
@@ -419,11 +419,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="%0." xfId="4"/>
@@ -473,7 +474,31 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -795,35 +820,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>B2</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>B3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>D2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>F2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -19981,53 +20067,26 @@
 </easyPacket>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
task-32 Fix case 'not equal' and inhomogeneous types and Test more cases
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
@@ -419,11 +419,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="%0." xfId="4"/>
@@ -473,7 +474,31 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -795,35 +820,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B3"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>B2</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>B3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>D2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>F2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -19981,53 +20067,26 @@
 </easyPacket>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Conditional formatting for blank cell (#42)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
@@ -48,12 +48,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00,"/>
-    <numFmt numFmtId="166" formatCode="#,##0,"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00,"/>
+    <numFmt numFmtId="168" formatCode="#,##0,"/>
+    <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -324,13 +324,13 @@
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -349,20 +349,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyFill="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0">
@@ -382,7 +382,7 @@
     <xf numFmtId="37" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -395,7 +395,7 @@
     <xf numFmtId="9" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="8" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="6" fillId="6" borderId="8" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
@@ -474,7 +474,76 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -823,7 +892,7 @@
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,23 +927,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="notEqual">
       <formula>B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>D2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>F2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#42 Added comments to xlsx
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_cell_is.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\GIT\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="195" yWindow="90" windowWidth="18390" windowHeight="7545" activeTab="1"/>
+    <workbookView xWindow="14720" yWindow="7640" windowWidth="20900" windowHeight="11660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="_TGK_HIDDEN" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,12 @@
     <definedName name="DOMESTIC">#REF!</definedName>
     <definedName name="INTL">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Template01</t>
   </si>
@@ -41,6 +44,24 @@
   </si>
   <si>
     <t>Foo</t>
+  </si>
+  <si>
+    <t>Not equals to 0</t>
+  </si>
+  <si>
+    <t>Conditional formatting on row (red background if condition true):</t>
+  </si>
+  <si>
+    <t>Equals to the cell above</t>
+  </si>
+  <si>
+    <t>NOT equals to the cell above</t>
+  </si>
+  <si>
+    <t>Equals to zero</t>
+  </si>
+  <si>
+    <t>Not equals to boolean FALSE</t>
   </si>
 </sst>
 </file>
@@ -55,7 +76,7 @@
     <numFmt numFmtId="168" formatCode="#,##0,"/>
     <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +180,13 @@
       <name val="Webdings"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -419,12 +447,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="%0." xfId="4"/>
@@ -444,8 +473,6 @@
     <cellStyle name="Bold+Italic" xfId="18"/>
     <cellStyle name="C_Amount_ACT" xfId="19"/>
     <cellStyle name="C_Head" xfId="20"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="2" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Date" xfId="21"/>
     <cellStyle name="Fill light blue" xfId="22"/>
     <cellStyle name="Formula" xfId="23"/>
@@ -453,7 +480,8 @@
     <cellStyle name="Hyperlink for amounts" xfId="25"/>
     <cellStyle name="Hyperlnk row header underlined bold" xfId="26"/>
     <cellStyle name="Middle Headers Centered" xfId="27"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Otsikko" xfId="3" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Placeholder" xfId="28"/>
     <cellStyle name="Placeholder Header Underlined bold" xfId="29"/>
     <cellStyle name="Placeholder_column_blank" xfId="30"/>
@@ -466,7 +494,8 @@
     <cellStyle name="Subtotal head row fill" xfId="37"/>
     <cellStyle name="Subtotal_amounts" xfId="38"/>
     <cellStyle name="TGK_TOC_PAGE_COLUMN" xfId="39"/>
-    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Valuutta" xfId="1" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Valuutta [0]" xfId="2" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Visual Check" xfId="40"/>
     <cellStyle name="Webdings" xfId="41"/>
     <cellStyle name="Webdings1" xfId="42"/>
@@ -474,56 +503,8 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="7">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -854,26 +835,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -889,15 +870,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="58.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -908,7 +897,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -919,45 +911,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="2"/>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="notEqual">
       <formula>B3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>D2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>F2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -985,15 +995,6 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -20151,6 +20152,15 @@
 </easyPacket>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
   <ds:schemaRefs/>
@@ -20164,13 +20174,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>